<commit_message>
Adding avg/stdev data to xlsx
</commit_message>
<xml_diff>
--- a/FF.xlsx
+++ b/FF.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
     <sheet name="Transactions" sheetId="2" r:id="rId2"/>
+    <sheet name="erik's stuff" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>team</t>
   </si>
@@ -104,13 +105,22 @@
   </si>
   <si>
     <t>Activate</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,16 +128,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -135,13 +189,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,16 +557,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -506,7 +642,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -544,7 +680,7 @@
         <v>122.6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -582,7 +718,7 @@
         <v>107.8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -620,7 +756,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -658,7 +794,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -696,7 +832,7 @@
         <v>115.3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -734,7 +870,7 @@
         <v>51.8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -772,7 +908,7 @@
         <v>106.9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -810,7 +946,7 @@
         <v>81.7</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -848,7 +984,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -886,7 +1022,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -930,19 +1066,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +1095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -976,7 +1112,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -993,7 +1129,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1010,7 +1146,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1027,7 +1163,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1044,7 +1180,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1061,7 +1197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1078,7 +1214,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1095,7 +1231,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1112,7 +1248,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1129,7 +1265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1146,7 +1282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1161,6 +1297,169 @@
       </c>
       <c r="E13">
         <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474F5339-554F-4882-A23F-D871D39F6732}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6">
+        <v>108.6</v>
+      </c>
+      <c r="C2" s="7">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9">
+        <v>101.1</v>
+      </c>
+      <c r="C3" s="10">
+        <v>11.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6">
+        <v>103.7</v>
+      </c>
+      <c r="C4" s="11">
+        <v>13.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="9">
+        <v>96.3</v>
+      </c>
+      <c r="C5" s="10">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="C6" s="11">
+        <v>17.11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="9">
+        <v>93.8</v>
+      </c>
+      <c r="C7" s="10">
+        <v>17.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6">
+        <v>99.6</v>
+      </c>
+      <c r="C8" s="11">
+        <v>17.690000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="9">
+        <v>98.2</v>
+      </c>
+      <c r="C9" s="10">
+        <v>18.29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="6">
+        <v>99.3</v>
+      </c>
+      <c r="C10" s="11">
+        <v>20.09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9">
+        <v>93.5</v>
+      </c>
+      <c r="C11" s="10">
+        <v>23.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6">
+        <v>92.7</v>
+      </c>
+      <c r="C12" s="11">
+        <v>26.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="9">
+        <v>108.9</v>
+      </c>
+      <c r="C13" s="7">
+        <v>26.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>